<commit_message>
Recuperando estado de salud
</commit_message>
<xml_diff>
--- a/Documentacion/Datos de prueba.xlsx
+++ b/Documentacion/Datos de prueba.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orlan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ISIL DESARROLLO DE SOTFWARE\DESARROLLO DE APLICACIONES\Proyecto_Institutec_2\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE394EC-DAE7-439C-B5D0-30309ED882E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2A8745-C23A-459E-B42A-6B8104ACB156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="GrupoInstitutec" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Profesor</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Servicio CRUD</t>
-  </si>
-  <si>
-    <t>Servicio Operaciones</t>
   </si>
   <si>
     <t>Insertar</t>
@@ -399,30 +396,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>EliminarAlumno:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
--strCodigo: A001 al A020</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>ListarAlumno:</t>
     </r>
     <r>
@@ -521,30 +494,6 @@
 ApeMat: Martinez
 SexoPr: M
 IdUbigeo: 140122, 140106,140128, 140129</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">EliminarProfesor: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
--strCodigo: P020-P024</t>
     </r>
   </si>
   <si>
@@ -591,6 +540,76 @@
 CodCar: CA01 A CA20
 FotoAlum: img 
 direcc: dirección</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EliminarAlumno:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+-strCodigo:                                        A001,A022,A023</t>
+    </r>
+  </si>
+  <si>
+    <t>Datos</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">EliminarProfesor: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+-strCodigo: P025</t>
+    </r>
+  </si>
+  <si>
+    <t>ListarProfesorEspecialidad</t>
+  </si>
+  <si>
+    <t>ListarAlumnoNRC</t>
+  </si>
+  <si>
+    <t>Servicio Operaciones   Consultas de negocio</t>
+  </si>
+  <si>
+    <t>NRC059,NRC060,NRC070
+NRC059,NRC061,NRC063</t>
+  </si>
+  <si>
+    <t>1 ,2,3,4,5,6,7,8,9,10</t>
+  </si>
+  <si>
+    <t>Consulta de negocio</t>
   </si>
 </sst>
 </file>
@@ -653,7 +672,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -700,11 +719,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -742,6 +774,42 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1023,36 +1091,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:H8"/>
+  <dimension ref="B2:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1"/>
-    <col min="2" max="2" width="26.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="35.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" style="1" customWidth="1"/>
     <col min="4" max="8" width="24.28515625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="233.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1063,19 +1133,19 @@
         <v>0</v>
       </c>
       <c r="D3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="G3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="262.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1084,19 +1154,19 @@
         <v>1</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>21</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="216.75" x14ac:dyDescent="0.2">
@@ -1105,19 +1175,19 @@
         <v>2</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="127.5" x14ac:dyDescent="0.2">
@@ -1127,40 +1197,80 @@
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="B7" s="12"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B8" s="13"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-    </row>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="15"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="24"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="15"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="25"/>
+    </row>
+    <row r="15" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="15"/>
+      <c r="C15" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="15"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="21"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="16"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="22"/>
+    </row>
+    <row r="20" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="7">
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="B12:B17"/>
+    <mergeCell ref="C15:C17"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="B7:B8"/>
   </mergeCells>

</xml_diff>

<commit_message>
Agregando servicio ObtenerCarreraXGenero y actulizando excel
</commit_message>
<xml_diff>
--- a/Documentacion/Datos de prueba.xlsx
+++ b/Documentacion/Datos de prueba.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\desarrolloDeAplicaciones2\Proyecto_Institutec_2\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ISIL DESARROLLO DE SOTFWARE\DESARROLLO DE APLICACIONES\Proyecto_Institutec_2\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD96B6EB-9038-4E1E-A3F8-C87480E07C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB492AEA-CAAA-443D-B315-CD9AE22697A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Curso</t>
   </si>
@@ -610,6 +610,18 @@
   </si>
   <si>
     <t>Seccion(OBLIGATORIO)</t>
+  </si>
+  <si>
+    <t>ObtenerCarreraXGenero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matriculados por sección </t>
+  </si>
+  <si>
+    <t>Curso que dicta el profesor</t>
+  </si>
+  <si>
+    <t>Opcional ver Todos los cursos de alumno</t>
   </si>
 </sst>
 </file>
@@ -742,7 +754,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -772,6 +784,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -799,25 +817,7 @@
     <xf numFmtId="16" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1100,18 +1100,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:H20"/>
+  <dimension ref="B2:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1"/>
-    <col min="2" max="2" width="35.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="28.85546875" style="1" customWidth="1"/>
     <col min="4" max="8" width="24.28515625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="11.42578125" style="1"/>
@@ -1135,10 +1135,10 @@
       </c>
     </row>
     <row r="3" spans="2:8" ht="233.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="11" t="s">
         <v>33</v>
       </c>
       <c r="D3" s="10" t="s">
@@ -1158,8 +1158,8 @@
       </c>
     </row>
     <row r="4" spans="2:8" ht="262.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="23"/>
-      <c r="C4" s="26" t="s">
+      <c r="B4" s="12"/>
+      <c r="C4" s="11" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="6" t="s">
@@ -1179,8 +1179,8 @@
       </c>
     </row>
     <row r="5" spans="2:8" ht="216.75" x14ac:dyDescent="0.2">
-      <c r="B5" s="23"/>
-      <c r="C5" s="26" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="11" t="s">
         <v>35</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -1200,7 +1200,7 @@
       </c>
     </row>
     <row r="6" spans="2:8" ht="127.5" x14ac:dyDescent="0.2">
-      <c r="B6" s="23"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="5" t="s">
         <v>0</v>
       </c>
@@ -1218,13 +1218,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="24"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="25"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="22" t="s">
+        <v>29</v>
+      </c>
       <c r="C11" s="3" t="s">
         <v>32</v>
       </c>
@@ -1233,54 +1230,84 @@
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="11" t="s">
+      <c r="B12" s="22"/>
+      <c r="C12" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="19" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="21"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="18"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="20"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="21"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="19"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="21"/>
     </row>
     <row r="15" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="21"/>
-      <c r="C15" s="11" t="s">
+      <c r="B15" s="22"/>
+      <c r="C15" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="16" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B16" s="21"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="15"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="17"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="22"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="16"/>
-    </row>
-    <row r="20" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="18"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="22"/>
+      <c r="C18" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="16"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="22"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="17"/>
+    </row>
+    <row r="20" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="22"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="18"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C22" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C23" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C24" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="B11:B20"/>
     <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C12:C14"/>
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="D12:D14"/>
-    <mergeCell ref="B12:B17"/>
     <mergeCell ref="C15:C17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>